<commit_message>
edit table lab 4
</commit_message>
<xml_diff>
--- a/МиТР/Lab_4/lab5.xlsx
+++ b/МиТР/Lab_4/lab5.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t xml:space="preserve">Частота (период) меток времени, </t>
   </si>
@@ -380,15 +380,6 @@
     <t>±100</t>
   </si>
   <si>
-    <t>d0</t>
-  </si>
-  <si>
-    <t>dкв</t>
-  </si>
-  <si>
-    <t>dзап</t>
-  </si>
-  <si>
     <t xml:space="preserve">Установлено </t>
   </si>
   <si>
@@ -643,13 +634,43 @@
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, м</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>с</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
         <vertAlign val="subscript"/>
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t xml:space="preserve"> </t>
+      <t>Т</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>S</t>
     </r>
     <r>
       <rPr>
@@ -670,22 +691,134 @@
   </si>
   <si>
     <r>
+      <t>d</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>Т</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+      </rPr>
+      <t>S</t>
+    </r>
+  </si>
+  <si>
+    <t>10^5</t>
+  </si>
+  <si>
+    <t>±0,0001</t>
+  </si>
+  <si>
+    <t>10^4</t>
+  </si>
+  <si>
+    <t>10^3</t>
+  </si>
+  <si>
+    <t>10^2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Установлено на шкале генератора</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Режим измерения частоты, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Symbol"/>
+      </rPr>
       <t>D</t>
     </r>
     <r>
       <rPr>
         <i/>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Т</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> =1  с</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Результат измерения и оценки погрешности</t>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> , Гц</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">x кГц</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Symbol"/>
       </rPr>
@@ -693,19 +826,19 @@
     </r>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>мс</t>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> Гц</t>
     </r>
   </si>
   <si>
@@ -716,16 +849,16 @@
       <rPr>
         <i/>
         <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>Т</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>f</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
         <color theme="1"/>
         <rFont val="Symbol"/>
       </rPr>
@@ -733,236 +866,173 @@
     </r>
   </si>
   <si>
-    <t>10^5</t>
-  </si>
-  <si>
-    <t>±0.0001</t>
-  </si>
-  <si>
-    <t>10^4</t>
-  </si>
-  <si>
-    <t>10^3</t>
-  </si>
-  <si>
-    <t>10^2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Установлено на шкале генератора</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Режим измерения частоты, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-      </rPr>
+    <t>n</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">x </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>макс</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">x </t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>мин</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>D</t>
     </r>
     <r>
       <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>зап</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>D</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t>кв</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve">, мс</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>nT</t>
+    </r>
+    <r>
+      <rPr>
         <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>t</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
+        <vertAlign val="subscript"/>
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t xml:space="preserve"> =1  с</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Результат измерения и оценки погрешности</t>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> , Гц</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">x кГц</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t>S</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve"> Гц</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>d</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>f</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Symbol"/>
-      </rPr>
-      <t>S</t>
-    </r>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">x </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>макс</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">x </t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>мин</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t>x</t>
     </r>
     <r>
@@ -971,109 +1041,21 @@
         <color theme="1"/>
         <rFont val="Times New Roman"/>
       </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>зап</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>кв</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t xml:space="preserve">, мс</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>nT</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <vertAlign val="subscript"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-      </rPr>
       <t xml:space="preserve">, с</t>
     </r>
-  </si>
-  <si>
-    <t>z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="6">
     <numFmt numFmtId="160" formatCode="0.0000"/>
-    <numFmt numFmtId="161" formatCode="0.00000"/>
+    <numFmt numFmtId="161" formatCode="0.000"/>
+    <numFmt numFmtId="162" formatCode="0.0"/>
+    <numFmt numFmtId="163" formatCode="0.00000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000000"/>
+    <numFmt numFmtId="165" formatCode="0.0000000000"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -1104,19 +1086,19 @@
       <sz val="12"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
+      <color theme="1" tint="0"/>
+      <sz val="12"/>
+    </font>
+    <font>
       <name val="Calibri"/>
       <i/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <name val="Anonymice Powerline"/>
-      <color theme="1"/>
-      <sz val="12"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1125,12 +1107,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor theme="9" tint="0.39997558519241921"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1214,21 +1202,6 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -1261,67 +1234,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color theme="1"/>
+      <top style="thin">
+        <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="medium">
-        <color theme="1"/>
-      </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1329,7 +1328,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="40">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1349,6 +1348,12 @@
     <xf fontId="1" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="2" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="2" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1358,61 +1363,82 @@
     <xf fontId="4" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="2" borderId="6" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="6" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="5" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="3" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="2" borderId="6" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="6" numFmtId="160" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="6" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="5" fillId="2" borderId="6" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="2" borderId="6" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="2" borderId="6" numFmtId="162" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf fontId="4" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="6" numFmtId="161" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="6" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="6" numFmtId="163" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="6" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="11" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="12" numFmtId="0" xfId="0" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf fontId="1" fillId="0" borderId="8" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf fontId="1" fillId="0" borderId="13" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="14" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf fontId="1" fillId="0" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf fontId="1" fillId="0" borderId="15" numFmtId="165" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="1" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1925,26 +1951,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100">
-      <selection activeCell="G31" activeCellId="0" sqref="G31"/>
+      <selection activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col bestFit="1" customWidth="1" min="2" max="2" width="12.85546875"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" width="15.42578125"/>
+    <col customWidth="1" min="3" max="3" width="11.28125"/>
+    <col customWidth="1" min="4" max="4" width="11.8515625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" width="28.7109375"/>
     <col bestFit="1" customWidth="1" min="6" max="6" width="13.7109375"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" width="13.85546875"/>
-    <col customWidth="1" min="8" max="8" width="11.421875"/>
-    <col customWidth="1" min="9" max="9" width="26.140625"/>
-    <col customWidth="1" min="10" max="10" width="20.00390625"/>
+    <col bestFit="1" customWidth="1" min="7" max="8" width="19.28515625"/>
+    <col bestFit="1" customWidth="1" min="9" max="9" width="20.28515625"/>
+    <col bestFit="1" customWidth="1" min="10" max="10" width="17.85546875"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" width="17.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="E1">
+    <row r="1" ht="18.75" customHeight="1"/>
+    <row r="2" ht="75" customHeight="1">
+      <c r="A2">
         <v>5.2000000000000002</v>
       </c>
-    </row>
-    <row r="2" ht="75" customHeight="1">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1969,53 +1996,52 @@
       </c>
     </row>
     <row r="4" ht="15">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="8">
         <v>100</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="8">
         <v>100</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="8">
         <v>100</v>
       </c>
     </row>
     <row r="5" ht="15">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="8">
         <v>1000</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="8">
         <v>1000</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="8">
         <v>1000</v>
       </c>
     </row>
     <row r="6" ht="15">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="8">
         <v>10000</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="8">
         <v>10000</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="8">
         <v>10000</v>
       </c>
     </row>
-    <row r="9" ht="15.75">
-      <c r="G9">
+    <row r="9" ht="15.75"/>
+    <row r="10" ht="15">
+      <c r="A10">
         <v>5.2999999999999998</v>
       </c>
-    </row>
-    <row r="10" ht="15">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
@@ -2033,19 +2059,19 @@
       <c r="B11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="G11" s="7" t="s">
+      <c r="G11" s="9" t="s">
         <v>14</v>
       </c>
     </row>
@@ -2059,17 +2085,21 @@
       <c r="D12" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="10">
-        <v>172.74420000000001</v>
-      </c>
-      <c r="G12" s="11">
+      <c r="F12" s="13">
+        <v>174.74420000000001</v>
+      </c>
+      <c r="G12" s="14">
+        <f>$J$12-F12</f>
         <v>0</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="I12" s="15" t="s">
         <v>18</v>
+      </c>
+      <c r="J12">
+        <v>174.74420000000001</v>
       </c>
     </row>
     <row r="13" ht="15">
@@ -2085,11 +2115,12 @@
       <c r="E13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="11">
-        <v>172.744</v>
-      </c>
-      <c r="G13" s="13">
-        <v>0.00020000000000000001</v>
+      <c r="F13" s="16">
+        <v>174.744</v>
+      </c>
+      <c r="G13" s="14">
+        <f>$J$12-F13</f>
+        <v>0.00020000000000663931</v>
       </c>
     </row>
     <row r="14" ht="15">
@@ -2105,14 +2136,15 @@
       <c r="E14" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F14" s="11">
-        <v>172.74000000000001</v>
-      </c>
-      <c r="G14" s="13">
-        <v>0.0041999999999999997</v>
-      </c>
-    </row>
-    <row r="15" ht="16.5">
+      <c r="F14" s="17">
+        <v>174.74000000000001</v>
+      </c>
+      <c r="G14" s="14">
+        <f>$J$12-F14</f>
+        <v>0.004199999999997317</v>
+      </c>
+    </row>
+    <row r="15" ht="15">
       <c r="B15" s="5" t="s">
         <v>24</v>
       </c>
@@ -2125,39 +2157,25 @@
       <c r="E15" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F15" s="11">
-        <v>172.69999999999999</v>
-      </c>
-      <c r="G15" s="13">
-        <v>0.044200000000000003</v>
-      </c>
-      <c r="I15" s="14" t="s">
+      <c r="F15" s="18">
+        <v>174.69999999999999</v>
+      </c>
+      <c r="G15" s="14">
+        <f>$J$12-F15</f>
+        <v>0.044200000000017781</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75"/>
+    <row r="19" ht="16.5">
+      <c r="A19">
+        <v>5.4000000000000004</v>
+      </c>
+      <c r="B19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="J15" s="14" t="s">
+      <c r="C19" s="20"/>
+      <c r="D19" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="K15" s="14" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" ht="14.25">
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-    </row>
-    <row r="18" ht="15.75">
-      <c r="K18">
-        <v>5.4000000000000004</v>
-      </c>
-    </row>
-    <row r="19" ht="16.5">
-      <c r="B19" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="17"/>
-      <c r="D19" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
@@ -2168,202 +2186,229 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20" ht="16.5">
-      <c r="B20" s="18" t="s">
-        <v>31</v>
+      <c r="B20" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="C20" s="6"/>
       <c r="D20" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
       <c r="G20" s="4"/>
       <c r="H20" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" ht="16.5">
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="F21" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="I21" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="J21" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H21" s="7" t="s">
+      <c r="K21" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I21" s="7" t="s">
+    </row>
+    <row r="22" ht="15">
+      <c r="B22" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="J21" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K21" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" ht="15">
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="6">
+      <c r="C22" s="8">
         <v>0.01</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="8">
         <v>0.01</v>
       </c>
-      <c r="E22" s="6">
+      <c r="E22" s="8">
         <v>0.0099000000000000008</v>
       </c>
       <c r="F22" s="6">
         <f t="shared" ref="F22:F25" si="0">(D22+E22)/2</f>
         <v>0.0099500000000000005</v>
       </c>
-      <c r="G22" s="20">
-        <f>(D22-E22)/2</f>
+      <c r="G22" s="24">
+        <f t="shared" ref="G22:G25" si="1">(D22-E22)/2</f>
         <v>4.9999999999999697e-05</v>
       </c>
-      <c r="H22" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I22" s="6">
-        <f>F22*10^(-6)</f>
+      <c r="H22" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I22" s="25">
+        <f t="shared" ref="I22:I25" si="2">F22*10^(-6)</f>
         <v>9.9499999999999998e-09</v>
       </c>
-      <c r="J22" s="6">
-        <f>I22+0.0001+G22</f>
+      <c r="J22" s="26">
+        <f t="shared" ref="J22:J25" si="3">I22+0.0001+G22</f>
         <v>0.00015000994999999972</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22" s="27">
+        <f t="shared" ref="K22:K25" si="4">(10^(-6)+(0.1*10^(-6)/(F22*10^(-3)))+0.003)</f>
+        <v>0.013051251256281406</v>
+      </c>
+      <c r="M22" s="28">
+        <f t="shared" ref="M22:M25" si="5">(10^(-6)+(0.003)/10+1/(10*(1/(0.1*10^(-6)))*F22*10^(-3)))*100</f>
+        <v>0.13060251256281408</v>
+      </c>
     </row>
     <row r="23" ht="15">
-      <c r="B23" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="6">
+      <c r="B23" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="8">
         <v>0.10000000000000001</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="8">
         <v>0.099500000000000005</v>
       </c>
-      <c r="E23" s="6">
+      <c r="E23" s="8">
         <v>0.099299999999999999</v>
       </c>
       <c r="F23" s="6">
         <f t="shared" si="0"/>
         <v>0.099400000000000002</v>
       </c>
-      <c r="G23" s="20">
-        <f t="shared" ref="G23:G25" si="1">(D23-E23)/2</f>
+      <c r="G23" s="24">
+        <f t="shared" si="1"/>
         <v>0.00010000000000000286</v>
       </c>
-      <c r="H23" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I23" s="6">
-        <f>F23*10^(-6)</f>
+      <c r="H23" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="25">
+        <f t="shared" si="2"/>
         <v>9.9400000000000003e-08</v>
       </c>
-      <c r="J23" s="6">
-        <f>I23+0.0001+G23</f>
+      <c r="J23" s="26">
+        <f t="shared" si="3"/>
         <v>0.00020009940000000287</v>
       </c>
-      <c r="K23" s="6"/>
+      <c r="K23" s="27">
+        <f t="shared" si="4"/>
+        <v>0.0040070362173038228</v>
+      </c>
+      <c r="M23" s="28">
+        <f t="shared" si="5"/>
+        <v>0.040160362173038235</v>
+      </c>
     </row>
     <row r="24" ht="15">
-      <c r="B24" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="6">
+      <c r="B24" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="8">
         <v>1</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="8">
         <v>0.99539999999999995</v>
       </c>
-      <c r="E24" s="6">
+      <c r="E24" s="8">
         <v>0.99519999999999997</v>
       </c>
       <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>0.99529999999999996</v>
       </c>
-      <c r="G24" s="20">
+      <c r="G24" s="24">
         <f t="shared" si="1"/>
         <v>9.9999999999988987e-05</v>
       </c>
-      <c r="H24" s="21" t="s">
+      <c r="H24" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I24" s="25">
+        <f t="shared" si="2"/>
+        <v>9.9529999999999981e-07</v>
+      </c>
+      <c r="J24" s="26">
+        <f t="shared" si="3"/>
+        <v>0.00020099529999998897</v>
+      </c>
+      <c r="K24" s="27">
+        <f t="shared" si="4"/>
+        <v>0.0031014722194313274</v>
+      </c>
+      <c r="M24" s="28">
+        <f t="shared" si="5"/>
+        <v>0.031104722194313275</v>
+      </c>
+    </row>
+    <row r="25" ht="15">
+      <c r="B25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I24" s="6">
-        <f>F24*10^(-6)</f>
-        <v>9.9529999999999981e-07</v>
-      </c>
-      <c r="J24" s="6">
-        <f>I24+0.0001+G24</f>
-        <v>0.00020099529999998897</v>
-      </c>
-      <c r="K24" s="6"/>
-    </row>
-    <row r="25" ht="15">
-      <c r="B25" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="6">
+      <c r="C25" s="8">
         <v>10</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="8">
         <v>9.9472000000000005</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="8">
         <v>9.9441000000000006</v>
       </c>
       <c r="F25" s="6">
         <f t="shared" si="0"/>
         <v>9.9456500000000005</v>
       </c>
-      <c r="G25" s="20">
+      <c r="G25" s="24">
         <f t="shared" si="1"/>
         <v>0.0015499999999999403</v>
       </c>
-      <c r="H25" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="I25" s="6">
-        <f>F25*10^(-6)</f>
+      <c r="H25" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="25">
+        <f t="shared" si="2"/>
         <v>9.9456500000000002e-06</v>
       </c>
-      <c r="J25" s="6">
-        <f>I25+0.0001+G25</f>
+      <c r="J25" s="26">
+        <f t="shared" si="3"/>
         <v>0.0016599456499999403</v>
       </c>
-      <c r="K25" s="6"/>
-    </row>
-    <row r="27" ht="15.75">
-      <c r="E27">
+      <c r="K25" s="27">
+        <f t="shared" si="4"/>
+        <v>0.0030110546470064805</v>
+      </c>
+      <c r="M25" s="28">
+        <f t="shared" si="5"/>
+        <v>0.030200546470064808</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75"/>
+    <row r="28" ht="35.25" customHeight="1">
+      <c r="A28">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="28" ht="35.25" customHeight="1">
       <c r="B28" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="4"/>
@@ -2371,43 +2416,47 @@
     <row r="29" ht="31.5" customHeight="1">
       <c r="B29" s="5"/>
       <c r="C29" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="4"/>
     </row>
     <row r="30" ht="17.25">
-      <c r="B30" s="19" t="s">
+      <c r="B30" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="9" t="s">
         <v>52</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E30" s="7" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="31" ht="15">
       <c r="B31" s="5">
         <v>100</v>
       </c>
-      <c r="C31" s="22">
+      <c r="C31" s="6">
         <v>0.10000000000000001</v>
       </c>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
-    </row>
-    <row r="34" ht="15.75">
-      <c r="I34">
+      <c r="D31" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" s="6">
+        <f>10^(-6)+(1/(100*1))</f>
+        <v>0.010000999999999999</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75"/>
+    <row r="35" ht="16.5">
+      <c r="A35">
         <v>5.5999999999999996</v>
       </c>
-    </row>
-    <row r="35" ht="16.5">
-      <c r="B35" s="23" t="s">
-        <v>56</v>
+      <c r="B35" s="29" t="s">
+        <v>53</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>8</v>
@@ -2421,133 +2470,134 @@
       <c r="H35" s="3"/>
       <c r="I35" s="4"/>
     </row>
-    <row r="36" ht="30">
-      <c r="B36" s="19"/>
-      <c r="C36" s="9" t="s">
+    <row r="36" ht="16.5">
+      <c r="B36" s="22"/>
+      <c r="C36" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D36" s="9" t="s">
+      <c r="G36" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="I36" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="G36" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="I36" s="9" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="37" ht="15">
-      <c r="B37" s="24">
+      <c r="B37" s="1">
         <v>1</v>
       </c>
-      <c r="C37" s="25">
+      <c r="C37" s="30">
         <v>32.240099999999998</v>
       </c>
-      <c r="D37" s="25">
+      <c r="D37" s="30">
         <v>32.236699999999999</v>
       </c>
-      <c r="E37" s="25">
-        <f>(C37+D37)/2</f>
+      <c r="E37" s="31">
+        <f t="shared" ref="E37:E38" si="6">(C37+D37)/2</f>
         <v>32.238399999999999</v>
       </c>
-      <c r="F37" s="25">
-        <f>(C37-D37)/2</f>
+      <c r="F37" s="31">
+        <f t="shared" ref="F37:F38" si="7">(C37-D37)/2</f>
         <v>0.0016999999999995907</v>
       </c>
-      <c r="G37" s="25">
-        <f>10^(-6)*E37</f>
+      <c r="G37" s="32">
+        <f t="shared" ref="G37:G38" si="8">10^(-6)*E37</f>
         <v>3.22384e-05</v>
       </c>
-      <c r="H37" s="25">
-        <f>0.0001</f>
-        <v>0.0001</v>
-      </c>
-      <c r="I37" s="26">
-        <f>B37*E37*10^(-3)</f>
+      <c r="H37" s="31">
+        <f>(0.1*10^(-6)/B37)*1000</f>
+        <v>9.9999999999999991e-05</v>
+      </c>
+      <c r="I37" s="31">
+        <f t="shared" ref="I37:I38" si="9">B37*E37*10^(-3)</f>
         <v>0.0322384</v>
       </c>
     </row>
     <row r="38" ht="15">
-      <c r="B38" s="27">
+      <c r="B38" s="33">
         <v>10</v>
       </c>
-      <c r="C38" s="28">
+      <c r="C38" s="34">
         <v>32.239130000000003</v>
       </c>
-      <c r="D38" s="28">
+      <c r="D38" s="34">
         <v>32.237369999999999</v>
       </c>
-      <c r="E38" s="25">
-        <f>(C38+D38)/2</f>
+      <c r="E38" s="35">
+        <f t="shared" si="6"/>
         <v>32.238250000000001</v>
       </c>
-      <c r="F38" s="25">
-        <f>(C38-D38)/2</f>
+      <c r="F38" s="35">
+        <f t="shared" si="7"/>
         <v>0.00088000000000221235</v>
       </c>
-      <c r="G38" s="25">
-        <f>10^(-6)*E38</f>
+      <c r="G38" s="36">
+        <f t="shared" si="8"/>
         <v>3.2238250000000003e-05</v>
       </c>
-      <c r="H38" s="28">
-        <f>0.0001/B38</f>
+      <c r="H38" s="37">
+        <f>0.1*10^(-6)/B38*1000</f>
         <v>1.0000000000000001e-05</v>
       </c>
-      <c r="I38" s="26">
-        <f>B38*E38*10^(-3)</f>
+      <c r="I38" s="38">
+        <f t="shared" si="9"/>
         <v>0.32238250000000002</v>
       </c>
     </row>
     <row r="39" ht="15">
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30" t="s">
-        <v>64</v>
-      </c>
+      <c r="B39" s="28"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="39"/>
+      <c r="H39" s="39"/>
+      <c r="I39" s="39"/>
     </row>
     <row r="40" ht="15">
-      <c r="B40" s="29"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
+      <c r="B40" s="28"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="39"/>
+      <c r="E40">
+        <f>F38/F37</f>
+        <v>0.51764705882495543</v>
+      </c>
+      <c r="F40" s="39"/>
+      <c r="G40" s="39"/>
+      <c r="H40" s="39"/>
+      <c r="I40" s="39"/>
     </row>
     <row r="41" ht="15">
-      <c r="B41" s="29"/>
-      <c r="C41" s="30"/>
-      <c r="D41" s="30"/>
-      <c r="E41" s="30"/>
-      <c r="F41" s="30"/>
-      <c r="G41" s="30"/>
-      <c r="H41" s="30"/>
-      <c r="I41" s="30"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="39"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="39"/>
+      <c r="H41" s="39"/>
+      <c r="I41" s="39"/>
     </row>
     <row r="42" ht="15">
-      <c r="B42" s="29"/>
-      <c r="C42" s="30"/>
-      <c r="D42" s="30"/>
-      <c r="E42" s="30"/>
-      <c r="F42" s="30"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+      <c r="I42" s="39"/>
     </row>
   </sheetData>
   <mergeCells count="13">

</xml_diff>